<commit_message>
Improved the model preformances
</commit_message>
<xml_diff>
--- a/Analysis and Models/Results.xlsx
+++ b/Analysis and Models/Results.xlsx
@@ -8,18 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usmanali/Uwindsor/Forth/Project/Analysis and Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49D9E512-8FC5-EA41-9734-63EC8B351E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F09802-5863-834C-9C14-4925AA2458E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{E4F4B0A7-86E0-A44A-9275-35D290469FE2}"/>
+    <workbookView xWindow="13900" yWindow="740" windowWidth="13620" windowHeight="16740" xr2:uid="{E4F4B0A7-86E0-A44A-9275-35D290469FE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Results!$A$2:$B$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Results!$C$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Results!$C$2:$C$21</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
   <si>
     <t>Year</t>
   </si>
@@ -55,31 +50,43 @@
     <t>Pred</t>
   </si>
   <si>
-    <t>Virutal Reality</t>
-  </si>
-  <si>
-    <t>Argumented Reality</t>
-  </si>
-  <si>
     <t>AI</t>
   </si>
   <si>
     <t>Quantum Computing</t>
   </si>
   <si>
-    <t>Internet of Things</t>
-  </si>
-  <si>
-    <t>growing - 2</t>
-  </si>
-  <si>
-    <t>full - 3</t>
-  </si>
-  <si>
-    <t>emerging - 1</t>
-  </si>
-  <si>
-    <t>Burst - 0</t>
+    <t>Physcial Credit Cards</t>
+  </si>
+  <si>
+    <t>Cloud Banking</t>
+  </si>
+  <si>
+    <t>Robotic Process Automation</t>
+  </si>
+  <si>
+    <t>Digital Wallets</t>
+  </si>
+  <si>
+    <t>Mobile Banking</t>
+  </si>
+  <si>
+    <t>BlockChain</t>
+  </si>
+  <si>
+    <t>2: 'Established', 1: 'Emerging', 3: 'Growing', 0: 'Decline'</t>
+  </si>
+  <si>
+    <t>Growing- 3</t>
+  </si>
+  <si>
+    <t>Established - 4</t>
+  </si>
+  <si>
+    <t>Decline - 1</t>
+  </si>
+  <si>
+    <t>Emerging - 2</t>
   </si>
 </sst>
 </file>
@@ -148,10 +155,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,20 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{968E2727-8FA6-CF42-87CF-966C4990576D}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -498,49 +502,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>45658</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>45658</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>45658</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>45658</v>
       </c>
@@ -548,13 +552,16 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>45658</v>
       </c>
@@ -562,220 +569,276 @@
         <v>8</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>45658</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>45658</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>45658</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>46023</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>46023</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>46023</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>46023</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>46023</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
-        <v>46388</v>
+        <v>46023</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
-        <v>46388</v>
+        <v>46023</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>46388</v>
+        <v>46023</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>46023</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>46388</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
       <c r="D15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>46023</v>
+      </c>
+      <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>46388</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
-        <v>46753</v>
+        <v>46023</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
-        <v>46753</v>
+        <v>46388</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
-        <v>46753</v>
+        <v>46388</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
-        <v>46753</v>
+        <v>46388</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
-        <v>46753</v>
+        <v>46388</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>46388</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>46388</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>46388</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>46388</v>
+      </c>
+      <c r="B25" t="s">
         <v>10</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>